<commit_message>
updated exercise2 results, tests and presence
</commit_message>
<xml_diff>
--- a/Oceny.xlsx
+++ b/Oceny.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="68">
   <si>
     <t>Jablonski Mateusz</t>
   </si>
@@ -219,6 +219,15 @@
   </si>
   <si>
     <t>####</t>
+  </si>
+  <si>
+    <t>start_thread</t>
+  </si>
+  <si>
+    <t>pro_con</t>
+  </si>
+  <si>
+    <t>counter</t>
   </si>
 </sst>
 </file>
@@ -481,7 +490,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$P$5</c:f>
+              <c:f>Sheet1!$S$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -552,7 +561,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$P$6:$P$19</c:f>
+              <c:f>Sheet1!$S$6:$S$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
@@ -586,7 +595,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$Q$5</c:f>
+              <c:f>Sheet1!$T$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -657,7 +666,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$Q$6:$Q$19</c:f>
+              <c:f>Sheet1!$T$6:$T$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
@@ -1459,7 +1468,7 @@
       <xdr:rowOff>14286</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>581025</xdr:colOff>
       <xdr:row>35</xdr:row>
       <xdr:rowOff>38099</xdr:rowOff>
@@ -1747,10 +1756,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:AO21"/>
+  <dimension ref="A4:AR21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S25" sqref="S25"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -1763,64 +1772,65 @@
     <col min="6" max="6" width="9.140625" customWidth="1"/>
     <col min="7" max="11" width="9.140625" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="12" max="12" width="9.140625" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="9.85546875" customWidth="1"/>
-    <col min="15" max="15" width="11.7109375" customWidth="1"/>
-    <col min="18" max="31" width="9.140625" customWidth="1" outlineLevel="1"/>
-    <col min="32" max="32" width="9.5703125" customWidth="1" outlineLevel="1"/>
-    <col min="33" max="33" width="35.5703125" customWidth="1"/>
-    <col min="34" max="35" width="17.5703125" customWidth="1"/>
-    <col min="36" max="37" width="16.42578125" customWidth="1"/>
-    <col min="38" max="38" width="16.7109375" customWidth="1"/>
+    <col min="13" max="15" width="9.140625" customWidth="1" outlineLevel="1"/>
+    <col min="17" max="17" width="9.85546875" customWidth="1"/>
+    <col min="18" max="18" width="11.7109375" customWidth="1"/>
+    <col min="21" max="34" width="9.140625" customWidth="1" outlineLevel="1"/>
+    <col min="35" max="35" width="9.5703125" customWidth="1" outlineLevel="1"/>
+    <col min="36" max="36" width="35.5703125" customWidth="1"/>
+    <col min="37" max="38" width="17.5703125" customWidth="1"/>
+    <col min="39" max="40" width="16.42578125" customWidth="1"/>
+    <col min="41" max="41" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="R4">
-        <v>1</v>
-      </c>
-      <c r="S4">
+    <row r="4" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="U4">
+        <v>1</v>
+      </c>
+      <c r="V4">
         <v>2</v>
       </c>
-      <c r="T4">
+      <c r="W4">
         <v>3</v>
       </c>
-      <c r="U4">
+      <c r="X4">
         <v>4</v>
       </c>
-      <c r="V4">
+      <c r="Y4">
         <v>5</v>
       </c>
-      <c r="W4">
+      <c r="Z4">
         <v>6</v>
       </c>
-      <c r="X4">
+      <c r="AA4">
         <v>7</v>
       </c>
-      <c r="Y4">
+      <c r="AB4">
         <v>8</v>
       </c>
-      <c r="Z4">
+      <c r="AC4">
         <v>9</v>
       </c>
-      <c r="AA4">
+      <c r="AD4">
         <v>10</v>
       </c>
-      <c r="AB4">
+      <c r="AE4">
         <v>11</v>
       </c>
-      <c r="AC4">
+      <c r="AF4">
         <v>12</v>
       </c>
-      <c r="AD4">
+      <c r="AG4">
         <v>13</v>
       </c>
-      <c r="AE4">
+      <c r="AH4">
         <v>14</v>
       </c>
-      <c r="AF4">
+      <c r="AI4">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>61</v>
       </c>
@@ -1858,103 +1868,112 @@
         <v>5</v>
       </c>
       <c r="M5" t="s">
+        <v>65</v>
+      </c>
+      <c r="N5" t="s">
+        <v>67</v>
+      </c>
+      <c r="O5" t="s">
+        <v>66</v>
+      </c>
+      <c r="P5" t="s">
         <v>30</v>
       </c>
-      <c r="N5" t="s">
+      <c r="Q5" t="s">
         <v>6</v>
       </c>
-      <c r="O5" t="s">
+      <c r="R5" t="s">
         <v>7</v>
       </c>
-      <c r="P5" t="s">
+      <c r="S5" t="s">
         <v>62</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="T5" t="s">
         <v>45</v>
       </c>
-      <c r="R5">
+      <c r="U5">
         <v>22.02</v>
       </c>
-      <c r="S5">
+      <c r="V5">
         <v>1.03</v>
       </c>
-      <c r="T5">
+      <c r="W5">
         <v>15.03</v>
       </c>
-      <c r="U5">
+      <c r="X5">
         <v>22.03</v>
       </c>
-      <c r="V5">
+      <c r="Y5">
         <v>29.03</v>
       </c>
-      <c r="W5">
+      <c r="Z5">
         <v>5.04</v>
       </c>
-      <c r="X5">
+      <c r="AA5">
         <v>12.04</v>
       </c>
-      <c r="Y5">
+      <c r="AB5">
         <v>19.04</v>
       </c>
-      <c r="Z5">
+      <c r="AC5">
         <v>26.04</v>
       </c>
-      <c r="AA5">
+      <c r="AD5">
         <v>3.05</v>
       </c>
-      <c r="AB5">
+      <c r="AE5">
         <v>10.050000000000001</v>
       </c>
-      <c r="AC5">
+      <c r="AF5">
         <v>17.05</v>
       </c>
-      <c r="AD5">
+      <c r="AG5">
         <v>24.05</v>
       </c>
-      <c r="AE5">
+      <c r="AH5">
         <v>31.05</v>
       </c>
-      <c r="AF5" t="s">
+      <c r="AI5" t="s">
         <v>9</v>
       </c>
-      <c r="AG5" t="s">
+      <c r="AJ5" t="s">
         <v>10</v>
       </c>
-      <c r="AH5" t="s">
+      <c r="AK5" t="s">
         <v>46</v>
       </c>
-      <c r="AI5" t="s">
+      <c r="AL5" t="s">
         <v>51</v>
       </c>
-      <c r="AJ5" t="s">
+      <c r="AM5" t="s">
         <v>53</v>
       </c>
-      <c r="AK5" t="s">
+      <c r="AN5" t="s">
         <v>54</v>
       </c>
-      <c r="AL5" t="s">
+      <c r="AO5" t="s">
         <v>16</v>
       </c>
-      <c r="AM5" t="s">
+      <c r="AP5" t="s">
         <v>17</v>
       </c>
-      <c r="AN5" t="s">
+      <c r="AQ5" t="s">
         <v>18</v>
       </c>
-      <c r="AO5" t="s">
+      <c r="AR5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>39</v>
       </c>
       <c r="C6">
-        <f>D6+Q6+P6</f>
+        <f>D6+T6+S6</f>
         <v>6</v>
       </c>
       <c r="D6">
-        <f>SUM(E6,F6,L6,M6,N6,O6)</f>
+        <f>SUM(E6,F6,L6,P6,Q6,R6)</f>
         <v>2</v>
       </c>
       <c r="E6">
@@ -1964,36 +1983,40 @@
         <f>SUM(G6:K6)</f>
         <v>0</v>
       </c>
-      <c r="Q6">
-        <f>SUM(R6:AF6)</f>
+      <c r="L6">
+        <f>SUM(M6:O6)</f>
+        <v>0</v>
+      </c>
+      <c r="T6">
+        <f>SUM(U6:AI6)</f>
         <v>4</v>
       </c>
-      <c r="R6">
-        <v>1</v>
-      </c>
-      <c r="S6">
-        <v>1</v>
-      </c>
-      <c r="T6">
-        <v>1</v>
-      </c>
       <c r="U6">
         <v>1</v>
       </c>
-      <c r="AG6" t="s">
+      <c r="V6">
+        <v>1</v>
+      </c>
+      <c r="W6">
+        <v>1</v>
+      </c>
+      <c r="X6">
+        <v>1</v>
+      </c>
+      <c r="AJ6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>38</v>
       </c>
       <c r="C7">
-        <f t="shared" ref="C7:C19" si="0">D7+Q7+P7</f>
+        <f t="shared" ref="C7:C19" si="0">D7+T7+S7</f>
         <v>13.5</v>
       </c>
       <c r="D7">
-        <f t="shared" ref="D7:D19" si="1">SUM(E7,F7,L7,M7,N7,O7)</f>
+        <f t="shared" ref="D7:D19" si="1">SUM(E7,F7,L7,P7,Q7,R7)</f>
         <v>6.5</v>
       </c>
       <c r="E7">
@@ -2018,22 +2041,17 @@
       <c r="K7">
         <v>0</v>
       </c>
-      <c r="P7">
-        <v>1</v>
-      </c>
-      <c r="Q7">
-        <f t="shared" ref="Q7:Q19" si="2">SUM(R7:AF7)</f>
+      <c r="L7">
+        <f t="shared" ref="L7:L19" si="2">SUM(M7:O7)</f>
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <v>1</v>
+      </c>
+      <c r="T7">
+        <f t="shared" ref="T7:T19" si="3">SUM(U7:AI7)</f>
         <v>6</v>
       </c>
-      <c r="R7">
-        <v>1</v>
-      </c>
-      <c r="S7">
-        <v>1</v>
-      </c>
-      <c r="T7">
-        <v>1</v>
-      </c>
       <c r="U7">
         <v>1</v>
       </c>
@@ -2043,20 +2061,29 @@
       <c r="W7">
         <v>1</v>
       </c>
-      <c r="AG7" t="s">
+      <c r="X7">
+        <v>1</v>
+      </c>
+      <c r="Y7">
+        <v>1</v>
+      </c>
+      <c r="Z7">
+        <v>1</v>
+      </c>
+      <c r="AJ7" t="s">
         <v>28</v>
       </c>
-      <c r="AH7" t="s">
+      <c r="AK7" t="s">
         <v>20</v>
       </c>
-      <c r="AI7" t="s">
+      <c r="AL7" t="s">
         <v>48</v>
       </c>
-      <c r="AJ7" t="s">
+      <c r="AM7" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>37</v>
       </c>
@@ -2072,30 +2099,34 @@
         <v>2</v>
       </c>
       <c r="F8">
-        <f t="shared" ref="F8:F19" si="3">SUM(G8:K8)</f>
-        <v>0</v>
-      </c>
-      <c r="Q8">
+        <f t="shared" ref="F8:F19" si="4">SUM(G8:K8)</f>
+        <v>0</v>
+      </c>
+      <c r="L8">
         <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T8">
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
-      <c r="R8">
-        <v>1</v>
-      </c>
-      <c r="S8">
-        <v>1</v>
-      </c>
-      <c r="T8">
-        <v>1</v>
-      </c>
       <c r="U8">
         <v>1</v>
       </c>
-      <c r="AG8" t="s">
+      <c r="V8">
+        <v>1</v>
+      </c>
+      <c r="W8">
+        <v>1</v>
+      </c>
+      <c r="X8">
+        <v>1</v>
+      </c>
+      <c r="AJ8" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -2108,30 +2139,34 @@
         <v>0</v>
       </c>
       <c r="F9">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="S9">
+        <v>1</v>
+      </c>
+      <c r="T9">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="P9">
-        <v>1</v>
-      </c>
-      <c r="Q9">
-        <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="S9">
-        <v>1</v>
-      </c>
-      <c r="T9">
-        <v>1</v>
-      </c>
-      <c r="U9">
-        <v>1</v>
-      </c>
       <c r="V9">
         <v>1</v>
       </c>
+      <c r="W9">
+        <v>1</v>
+      </c>
+      <c r="X9">
+        <v>1</v>
+      </c>
+      <c r="Y9">
+        <v>1</v>
+      </c>
     </row>
-    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -2144,30 +2179,34 @@
         <v>0</v>
       </c>
       <c r="F10">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="S10">
+        <v>1</v>
+      </c>
+      <c r="T10">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="P10">
-        <v>1</v>
-      </c>
-      <c r="Q10">
-        <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="S10">
-        <v>1</v>
-      </c>
-      <c r="T10">
-        <v>1</v>
-      </c>
       <c r="V10">
         <v>1</v>
       </c>
       <c r="W10">
         <v>1</v>
       </c>
+      <c r="Y10">
+        <v>1</v>
+      </c>
+      <c r="Z10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -2183,26 +2222,24 @@
         <v>2</v>
       </c>
       <c r="F11">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T11">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="G11">
-        <v>1</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="Q11">
-        <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="R11">
-        <v>1</v>
-      </c>
-      <c r="S11">
-        <v>1</v>
-      </c>
-      <c r="T11">
+      <c r="U11">
         <v>1</v>
       </c>
       <c r="V11">
@@ -2211,11 +2248,17 @@
       <c r="W11">
         <v>1</v>
       </c>
-      <c r="AG11" t="s">
+      <c r="Y11">
+        <v>1</v>
+      </c>
+      <c r="Z11">
+        <v>1</v>
+      </c>
+      <c r="AJ11" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -2228,27 +2271,31 @@
         <v>0</v>
       </c>
       <c r="F12">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T12">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="Q12">
-        <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="S12">
-        <v>1</v>
-      </c>
-      <c r="T12">
-        <v>1</v>
-      </c>
-      <c r="U12">
-        <v>1</v>
-      </c>
-      <c r="AG12" t="s">
+      <c r="V12">
+        <v>1</v>
+      </c>
+      <c r="W12">
+        <v>1</v>
+      </c>
+      <c r="X12">
+        <v>1</v>
+      </c>
+      <c r="AJ12" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -2264,7 +2311,7 @@
         <v>2</v>
       </c>
       <c r="F13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8.5</v>
       </c>
       <c r="G13">
@@ -2282,22 +2329,17 @@
       <c r="K13">
         <v>1</v>
       </c>
-      <c r="P13">
-        <v>1</v>
-      </c>
-      <c r="Q13">
+      <c r="L13">
         <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="S13">
+        <v>1</v>
+      </c>
+      <c r="T13">
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="R13">
-        <v>1</v>
-      </c>
-      <c r="S13">
-        <v>1</v>
-      </c>
-      <c r="T13">
-        <v>1</v>
-      </c>
       <c r="U13">
         <v>1</v>
       </c>
@@ -2307,17 +2349,26 @@
       <c r="W13">
         <v>1</v>
       </c>
-      <c r="AG13" t="s">
+      <c r="X13">
+        <v>1</v>
+      </c>
+      <c r="Y13">
+        <v>1</v>
+      </c>
+      <c r="Z13">
+        <v>1</v>
+      </c>
+      <c r="AJ13" t="s">
         <v>25</v>
       </c>
-      <c r="AI13" t="s">
+      <c r="AL13" t="s">
         <v>47</v>
       </c>
-      <c r="AJ13" t="s">
+      <c r="AM13" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>34</v>
       </c>
@@ -2333,33 +2384,37 @@
         <v>1</v>
       </c>
       <c r="F14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T14">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="Q14">
-        <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="R14">
-        <v>1</v>
-      </c>
-      <c r="S14">
-        <v>1</v>
-      </c>
-      <c r="T14">
-        <v>1</v>
-      </c>
       <c r="U14">
         <v>1</v>
       </c>
-      <c r="AG14" t="s">
+      <c r="V14">
+        <v>1</v>
+      </c>
+      <c r="W14">
+        <v>1</v>
+      </c>
+      <c r="X14">
+        <v>1</v>
+      </c>
+      <c r="AJ14" t="s">
         <v>15</v>
       </c>
-      <c r="AH14" t="s">
+      <c r="AK14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -2375,7 +2430,7 @@
         <v>2</v>
       </c>
       <c r="F15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
       <c r="G15">
@@ -2393,22 +2448,17 @@
       <c r="K15">
         <v>1</v>
       </c>
-      <c r="P15">
-        <v>1</v>
-      </c>
-      <c r="Q15">
+      <c r="L15">
         <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="S15">
+        <v>1</v>
+      </c>
+      <c r="T15">
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="R15">
-        <v>1</v>
-      </c>
-      <c r="S15">
-        <v>1</v>
-      </c>
-      <c r="T15">
-        <v>1</v>
-      </c>
       <c r="U15">
         <v>1</v>
       </c>
@@ -2418,17 +2468,26 @@
       <c r="W15">
         <v>1</v>
       </c>
-      <c r="AG15" t="s">
+      <c r="X15">
+        <v>1</v>
+      </c>
+      <c r="Y15">
+        <v>1</v>
+      </c>
+      <c r="Z15">
+        <v>1</v>
+      </c>
+      <c r="AJ15" t="s">
         <v>22</v>
       </c>
-      <c r="AI15" t="s">
+      <c r="AL15" t="s">
         <v>52</v>
       </c>
-      <c r="AJ15" t="s">
+      <c r="AM15" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -2444,7 +2503,7 @@
         <v>2</v>
       </c>
       <c r="F16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6.5</v>
       </c>
       <c r="G16">
@@ -2462,22 +2521,17 @@
       <c r="K16">
         <v>1</v>
       </c>
-      <c r="P16">
-        <v>1</v>
-      </c>
-      <c r="Q16">
+      <c r="L16">
         <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="S16">
+        <v>1</v>
+      </c>
+      <c r="T16">
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="R16">
-        <v>1</v>
-      </c>
-      <c r="S16">
-        <v>1</v>
-      </c>
-      <c r="T16">
-        <v>1</v>
-      </c>
       <c r="U16">
         <v>1</v>
       </c>
@@ -2487,17 +2541,26 @@
       <c r="W16">
         <v>1</v>
       </c>
-      <c r="AG16" t="s">
+      <c r="X16">
+        <v>1</v>
+      </c>
+      <c r="Y16">
+        <v>1</v>
+      </c>
+      <c r="Z16">
+        <v>1</v>
+      </c>
+      <c r="AJ16" t="s">
         <v>14</v>
       </c>
-      <c r="AI16" t="s">
+      <c r="AL16" t="s">
         <v>50</v>
       </c>
-      <c r="AJ16" t="s">
+      <c r="AM16" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>31</v>
       </c>
@@ -2513,7 +2576,7 @@
         <v>1</v>
       </c>
       <c r="F17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>9</v>
       </c>
       <c r="G17">
@@ -2531,19 +2594,14 @@
       <c r="K17">
         <v>1.5</v>
       </c>
-      <c r="Q17">
+      <c r="L17">
         <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T17">
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="R17">
-        <v>1</v>
-      </c>
-      <c r="S17">
-        <v>1</v>
-      </c>
-      <c r="T17">
-        <v>1</v>
-      </c>
       <c r="U17">
         <v>1</v>
       </c>
@@ -2553,17 +2611,26 @@
       <c r="W17">
         <v>1</v>
       </c>
-      <c r="AG17" t="s">
+      <c r="X17">
+        <v>1</v>
+      </c>
+      <c r="Y17">
+        <v>1</v>
+      </c>
+      <c r="Z17">
+        <v>1</v>
+      </c>
+      <c r="AJ17" t="s">
         <v>27</v>
       </c>
-      <c r="AH17" t="s">
+      <c r="AK17" t="s">
         <v>20</v>
       </c>
-      <c r="AI17" t="s">
+      <c r="AL17" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -2576,27 +2643,31 @@
         <v>0</v>
       </c>
       <c r="F18">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T18">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="Q18">
-        <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="S18">
-        <v>1</v>
-      </c>
-      <c r="T18">
-        <v>1</v>
-      </c>
-      <c r="U18">
-        <v>1</v>
-      </c>
       <c r="V18">
         <v>1</v>
       </c>
+      <c r="W18">
+        <v>1</v>
+      </c>
+      <c r="X18">
+        <v>1</v>
+      </c>
+      <c r="Y18">
+        <v>1</v>
+      </c>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>2</v>
       </c>
@@ -2612,7 +2683,7 @@
         <v>2</v>
       </c>
       <c r="F19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
       <c r="G19">
@@ -2630,40 +2701,44 @@
       <c r="K19">
         <v>0</v>
       </c>
-      <c r="P19">
-        <v>1</v>
-      </c>
-      <c r="Q19">
+      <c r="L19">
         <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="S19">
+        <v>1</v>
+      </c>
+      <c r="T19">
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="R19">
-        <v>1</v>
-      </c>
-      <c r="S19">
-        <v>1</v>
-      </c>
       <c r="U19">
         <v>1</v>
       </c>
       <c r="V19">
         <v>1</v>
       </c>
-      <c r="W19">
-        <v>1</v>
-      </c>
-      <c r="AG19" t="s">
+      <c r="X19">
+        <v>1</v>
+      </c>
+      <c r="Y19">
+        <v>1</v>
+      </c>
+      <c r="Z19">
+        <v>1</v>
+      </c>
+      <c r="AJ19" t="s">
         <v>11</v>
       </c>
-      <c r="AI19" t="s">
+      <c r="AL19" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="R21" t="s">
+    <row r="21" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="U21" t="s">
         <v>64</v>
       </c>
-      <c r="S21" t="s">
+      <c r="V21" t="s">
         <v>63</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated points for exercies and presence
</commit_message>
<xml_diff>
--- a/Oceny.xlsx
+++ b/Oceny.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Excel\UL\exercise0\exercise0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Excel\UL\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="69">
   <si>
     <t>Jablonski Mateusz</t>
   </si>
@@ -53,9 +53,6 @@
     <t>Ocena</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>Github</t>
   </si>
   <si>
@@ -215,19 +212,25 @@
     <t>Aktywnosc</t>
   </si>
   <si>
-    <t>Opis bonusowego zadania znajduje sie w readme exercise 2.</t>
-  </si>
-  <si>
-    <t>####</t>
-  </si>
-  <si>
-    <t>start_thread</t>
-  </si>
-  <si>
-    <t>pro_con</t>
+    <t>start</t>
   </si>
   <si>
     <t>counter</t>
+  </si>
+  <si>
+    <t>procon</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>https://github.com/walery1409</t>
+  </si>
+  <si>
+    <t>https://github.com/bioly1994</t>
+  </si>
+  <si>
+    <t>https://github.com/biedro94</t>
   </si>
 </sst>
 </file>
@@ -443,7 +446,7 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.5</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>2</c:v>
@@ -461,25 +464,25 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10.5</c:v>
+                  <c:v>24.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>8.5</c:v>
+                  <c:v>19.5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>10</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>9</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -490,7 +493,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$S$5</c:f>
+              <c:f>Sheet1!$T$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -561,7 +564,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$S$6:$S$19</c:f>
+              <c:f>Sheet1!$T$6:$T$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
@@ -595,7 +598,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$T$5</c:f>
+              <c:f>Sheet1!$U$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -666,51 +669,51 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$T$6:$T$19</c:f>
+              <c:f>Sheet1!$U$6:$U$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>6</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3</c:v>
-                </c:pt>
                 <c:pt idx="7">
-                  <c:v>6</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>6</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>5</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -726,11 +729,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="137105952"/>
-        <c:axId val="137107912"/>
+        <c:axId val="309333688"/>
+        <c:axId val="309334864"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="137105952"/>
+        <c:axId val="309333688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -773,7 +776,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="137107912"/>
+        <c:crossAx val="309334864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -781,7 +784,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="137107912"/>
+        <c:axId val="309334864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -832,7 +835,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="137105952"/>
+        <c:crossAx val="309333688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1468,7 +1471,7 @@
       <xdr:rowOff>14286</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>581025</xdr:colOff>
       <xdr:row>35</xdr:row>
       <xdr:rowOff>38099</xdr:rowOff>
@@ -1756,10 +1759,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:AR21"/>
+  <dimension ref="A4:AS19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -1772,76 +1775,77 @@
     <col min="6" max="6" width="9.140625" customWidth="1"/>
     <col min="7" max="11" width="9.140625" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="12" max="12" width="9.140625" customWidth="1" collapsed="1"/>
-    <col min="13" max="15" width="9.140625" customWidth="1" outlineLevel="1"/>
-    <col min="17" max="17" width="9.85546875" customWidth="1"/>
-    <col min="18" max="18" width="11.7109375" customWidth="1"/>
-    <col min="21" max="34" width="9.140625" customWidth="1" outlineLevel="1"/>
-    <col min="35" max="35" width="9.5703125" customWidth="1" outlineLevel="1"/>
-    <col min="36" max="36" width="35.5703125" customWidth="1"/>
-    <col min="37" max="38" width="17.5703125" customWidth="1"/>
-    <col min="39" max="40" width="16.42578125" customWidth="1"/>
-    <col min="41" max="41" width="16.7109375" customWidth="1"/>
+    <col min="13" max="16" width="9.140625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="17" max="17" width="9.140625" collapsed="1"/>
+    <col min="18" max="18" width="9.85546875" customWidth="1"/>
+    <col min="19" max="19" width="11.7109375" customWidth="1"/>
+    <col min="22" max="35" width="9.140625" customWidth="1" outlineLevel="1"/>
+    <col min="36" max="36" width="9.5703125" customWidth="1" outlineLevel="1"/>
+    <col min="37" max="37" width="35.5703125" customWidth="1"/>
+    <col min="38" max="39" width="17.5703125" customWidth="1"/>
+    <col min="40" max="41" width="16.42578125" customWidth="1"/>
+    <col min="42" max="42" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="U4">
-        <v>1</v>
-      </c>
+    <row r="4" spans="1:45" x14ac:dyDescent="0.25">
       <c r="V4">
+        <v>1</v>
+      </c>
+      <c r="W4">
         <v>2</v>
       </c>
-      <c r="W4">
+      <c r="X4">
         <v>3</v>
       </c>
-      <c r="X4">
+      <c r="Y4">
         <v>4</v>
       </c>
-      <c r="Y4">
+      <c r="Z4">
         <v>5</v>
       </c>
-      <c r="Z4">
+      <c r="AA4">
         <v>6</v>
       </c>
-      <c r="AA4">
+      <c r="AB4">
         <v>7</v>
       </c>
-      <c r="AB4">
+      <c r="AC4">
         <v>8</v>
       </c>
-      <c r="AC4">
+      <c r="AD4">
         <v>9</v>
       </c>
-      <c r="AD4">
+      <c r="AE4">
         <v>10</v>
       </c>
-      <c r="AE4">
+      <c r="AF4">
         <v>11</v>
       </c>
-      <c r="AF4">
+      <c r="AG4">
         <v>12</v>
       </c>
-      <c r="AG4">
+      <c r="AH4">
         <v>13</v>
       </c>
-      <c r="AH4">
+      <c r="AI4">
         <v>14</v>
       </c>
-      <c r="AI4">
+      <c r="AJ4">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E5" t="s">
         <v>3</v>
@@ -1850,130 +1854,133 @@
         <v>4</v>
       </c>
       <c r="G5" t="s">
+        <v>39</v>
+      </c>
+      <c r="H5" t="s">
         <v>40</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>41</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>42</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>43</v>
-      </c>
-      <c r="K5" t="s">
-        <v>44</v>
       </c>
       <c r="L5" t="s">
         <v>5</v>
       </c>
       <c r="M5" t="s">
+        <v>62</v>
+      </c>
+      <c r="N5" t="s">
+        <v>63</v>
+      </c>
+      <c r="O5" t="s">
+        <v>64</v>
+      </c>
+      <c r="P5" t="s">
         <v>65</v>
       </c>
-      <c r="N5" t="s">
-        <v>67</v>
-      </c>
-      <c r="O5" t="s">
-        <v>66</v>
-      </c>
-      <c r="P5" t="s">
-        <v>30</v>
-      </c>
       <c r="Q5" t="s">
+        <v>29</v>
+      </c>
+      <c r="R5" t="s">
         <v>6</v>
       </c>
-      <c r="R5" t="s">
+      <c r="S5" t="s">
         <v>7</v>
       </c>
-      <c r="S5" t="s">
-        <v>62</v>
-      </c>
       <c r="T5" t="s">
+        <v>61</v>
+      </c>
+      <c r="U5" t="s">
+        <v>44</v>
+      </c>
+      <c r="V5">
+        <v>22.02</v>
+      </c>
+      <c r="W5">
+        <v>1.03</v>
+      </c>
+      <c r="X5">
+        <v>15.03</v>
+      </c>
+      <c r="Y5">
+        <v>22.03</v>
+      </c>
+      <c r="Z5">
+        <v>29.03</v>
+      </c>
+      <c r="AA5">
+        <v>5.04</v>
+      </c>
+      <c r="AB5">
+        <v>12.04</v>
+      </c>
+      <c r="AC5">
+        <v>19.04</v>
+      </c>
+      <c r="AD5">
+        <v>26.04</v>
+      </c>
+      <c r="AE5">
+        <v>3.05</v>
+      </c>
+      <c r="AF5">
+        <v>10.050000000000001</v>
+      </c>
+      <c r="AG5">
+        <v>17.05</v>
+      </c>
+      <c r="AH5">
+        <v>24.05</v>
+      </c>
+      <c r="AI5">
+        <v>31.05</v>
+      </c>
+      <c r="AJ5">
+        <v>7.06</v>
+      </c>
+      <c r="AK5" t="s">
+        <v>9</v>
+      </c>
+      <c r="AL5" t="s">
         <v>45</v>
       </c>
-      <c r="U5">
-        <v>22.02</v>
-      </c>
-      <c r="V5">
-        <v>1.03</v>
-      </c>
-      <c r="W5">
-        <v>15.03</v>
-      </c>
-      <c r="X5">
-        <v>22.03</v>
-      </c>
-      <c r="Y5">
-        <v>29.03</v>
-      </c>
-      <c r="Z5">
-        <v>5.04</v>
-      </c>
-      <c r="AA5">
-        <v>12.04</v>
-      </c>
-      <c r="AB5">
-        <v>19.04</v>
-      </c>
-      <c r="AC5">
-        <v>26.04</v>
-      </c>
-      <c r="AD5">
-        <v>3.05</v>
-      </c>
-      <c r="AE5">
-        <v>10.050000000000001</v>
-      </c>
-      <c r="AF5">
-        <v>17.05</v>
-      </c>
-      <c r="AG5">
-        <v>24.05</v>
-      </c>
-      <c r="AH5">
-        <v>31.05</v>
-      </c>
-      <c r="AI5" t="s">
-        <v>9</v>
-      </c>
-      <c r="AJ5" t="s">
+      <c r="AM5" t="s">
+        <v>50</v>
+      </c>
+      <c r="AN5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AO5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AP5" t="s">
+        <v>15</v>
+      </c>
+      <c r="AQ5" t="s">
+        <v>16</v>
+      </c>
+      <c r="AR5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AS5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6">
+        <f t="shared" ref="C6:C19" si="0">D6+U6+T6</f>
         <v>10</v>
       </c>
-      <c r="AK5" t="s">
-        <v>46</v>
-      </c>
-      <c r="AL5" t="s">
-        <v>51</v>
-      </c>
-      <c r="AM5" t="s">
-        <v>53</v>
-      </c>
-      <c r="AN5" t="s">
-        <v>54</v>
-      </c>
-      <c r="AO5" t="s">
-        <v>16</v>
-      </c>
-      <c r="AP5" t="s">
-        <v>17</v>
-      </c>
-      <c r="AQ5" t="s">
-        <v>18</v>
-      </c>
-      <c r="AR5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C6">
-        <f>D6+T6+S6</f>
-        <v>6</v>
-      </c>
       <c r="D6">
-        <f>SUM(E6,F6,L6,P6,Q6,R6)</f>
+        <f t="shared" ref="D6:D19" si="1">SUM(E6,F6,L6,Q6,R6,S6)</f>
         <v>2</v>
       </c>
       <c r="E6">
@@ -1984,15 +1991,12 @@
         <v>0</v>
       </c>
       <c r="L6">
-        <f>SUM(M6:O6)</f>
+        <f>SUM(M6:P6)</f>
         <v>0</v>
       </c>
-      <c r="T6">
-        <f>SUM(U6:AI6)</f>
-        <v>4</v>
-      </c>
       <c r="U6">
-        <v>1</v>
+        <f>SUM(V6:AJ6)*2</f>
+        <v>8</v>
       </c>
       <c r="V6">
         <v>1</v>
@@ -2003,21 +2007,24 @@
       <c r="X6">
         <v>1</v>
       </c>
-      <c r="AJ6" t="s">
-        <v>13</v>
+      <c r="Y6">
+        <v>1</v>
+      </c>
+      <c r="AK6" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C7">
-        <f t="shared" ref="C7:C19" si="0">D7+T7+S7</f>
-        <v>13.5</v>
+        <f t="shared" si="0"/>
+        <v>33</v>
       </c>
       <c r="D7">
-        <f t="shared" ref="D7:D19" si="1">SUM(E7,F7,L7,P7,Q7,R7)</f>
-        <v>6.5</v>
+        <f t="shared" si="1"/>
+        <v>16</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -2042,18 +2049,24 @@
         <v>0</v>
       </c>
       <c r="L7">
-        <f t="shared" ref="L7:L19" si="2">SUM(M7:O7)</f>
-        <v>0</v>
-      </c>
-      <c r="S7">
-        <v>1</v>
+        <f t="shared" ref="L7:L19" si="2">SUM(M7:P7)</f>
+        <v>9.5</v>
+      </c>
+      <c r="M7">
+        <v>4</v>
+      </c>
+      <c r="N7">
+        <v>4</v>
+      </c>
+      <c r="O7">
+        <v>1.5</v>
       </c>
       <c r="T7">
-        <f t="shared" ref="T7:T19" si="3">SUM(U7:AI7)</f>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="U7">
-        <v>1</v>
+        <f t="shared" ref="U7:U19" si="3">SUM(V7:AJ7)*2</f>
+        <v>16</v>
       </c>
       <c r="V7">
         <v>1</v>
@@ -2070,26 +2083,35 @@
       <c r="Z7">
         <v>1</v>
       </c>
-      <c r="AJ7" t="s">
-        <v>28</v>
+      <c r="AA7">
+        <v>1</v>
+      </c>
+      <c r="AB7">
+        <v>1</v>
+      </c>
+      <c r="AC7">
+        <v>1</v>
       </c>
       <c r="AK7" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="AL7" t="s">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="AM7" t="s">
-        <v>57</v>
+        <v>47</v>
+      </c>
+      <c r="AN7" t="s">
+        <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C8">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D8">
         <f t="shared" si="1"/>
@@ -2106,12 +2128,9 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="T8">
+      <c r="U8">
         <f t="shared" si="3"/>
-        <v>4</v>
-      </c>
-      <c r="U8">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="V8">
         <v>1</v>
@@ -2122,17 +2141,20 @@
       <c r="X8">
         <v>1</v>
       </c>
-      <c r="AJ8" t="s">
-        <v>23</v>
+      <c r="Y8">
+        <v>1</v>
+      </c>
+      <c r="AK8" t="s">
+        <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>1</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D9">
         <f t="shared" si="1"/>
@@ -2146,15 +2168,12 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="S9">
-        <v>1</v>
-      </c>
       <c r="T9">
+        <v>1</v>
+      </c>
+      <c r="U9">
         <f t="shared" si="3"/>
-        <v>4</v>
-      </c>
-      <c r="V9">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="W9">
         <v>1</v>
@@ -2165,14 +2184,26 @@
       <c r="Y9">
         <v>1</v>
       </c>
+      <c r="Z9">
+        <v>1</v>
+      </c>
+      <c r="AB9">
+        <v>1</v>
+      </c>
+      <c r="AC9">
+        <v>1</v>
+      </c>
+      <c r="AK9" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="10" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C10">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D10">
         <f t="shared" si="1"/>
@@ -2186,33 +2217,36 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="S10">
-        <v>1</v>
-      </c>
       <c r="T10">
+        <v>1</v>
+      </c>
+      <c r="U10">
         <f t="shared" si="3"/>
-        <v>4</v>
-      </c>
-      <c r="V10">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="W10">
         <v>1</v>
       </c>
-      <c r="Y10">
+      <c r="X10">
         <v>1</v>
       </c>
       <c r="Z10">
         <v>1</v>
       </c>
+      <c r="AA10">
+        <v>1</v>
+      </c>
+      <c r="AK10" t="s">
+        <v>68</v>
+      </c>
     </row>
-    <row r="11" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>0</v>
       </c>
       <c r="C11">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D11">
         <f t="shared" si="1"/>
@@ -2235,12 +2269,9 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="T11">
+      <c r="U11">
         <f t="shared" si="3"/>
-        <v>5</v>
-      </c>
-      <c r="U11">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="V11">
         <v>1</v>
@@ -2248,23 +2279,29 @@
       <c r="W11">
         <v>1</v>
       </c>
-      <c r="Y11">
+      <c r="X11">
         <v>1</v>
       </c>
       <c r="Z11">
         <v>1</v>
       </c>
-      <c r="AJ11" t="s">
-        <v>21</v>
+      <c r="AA11">
+        <v>1</v>
+      </c>
+      <c r="AB11">
+        <v>1</v>
+      </c>
+      <c r="AK11" t="s">
+        <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C12">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D12">
         <f t="shared" si="1"/>
@@ -2278,12 +2315,9 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="T12">
+      <c r="U12">
         <f t="shared" si="3"/>
-        <v>3</v>
-      </c>
-      <c r="V12">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="W12">
         <v>1</v>
@@ -2291,21 +2325,24 @@
       <c r="X12">
         <v>1</v>
       </c>
-      <c r="AJ12" t="s">
-        <v>12</v>
+      <c r="Y12">
+        <v>1</v>
+      </c>
+      <c r="AK12" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C13">
         <f t="shared" si="0"/>
-        <v>17.5</v>
+        <v>41.5</v>
       </c>
       <c r="D13">
         <f t="shared" si="1"/>
-        <v>10.5</v>
+        <v>24.5</v>
       </c>
       <c r="E13">
         <v>2</v>
@@ -2331,17 +2368,26 @@
       </c>
       <c r="L13">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="S13">
-        <v>1</v>
+        <v>14</v>
+      </c>
+      <c r="M13">
+        <v>4.5</v>
+      </c>
+      <c r="N13">
+        <v>4.5</v>
+      </c>
+      <c r="O13">
+        <v>3</v>
+      </c>
+      <c r="P13">
+        <v>2</v>
       </c>
       <c r="T13">
+        <v>1</v>
+      </c>
+      <c r="U13">
         <f t="shared" si="3"/>
-        <v>6</v>
-      </c>
-      <c r="U13">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="V13">
         <v>1</v>
@@ -2358,23 +2404,32 @@
       <c r="Z13">
         <v>1</v>
       </c>
-      <c r="AJ13" t="s">
-        <v>25</v>
-      </c>
-      <c r="AL13" t="s">
-        <v>47</v>
+      <c r="AA13">
+        <v>1</v>
+      </c>
+      <c r="AB13">
+        <v>1</v>
+      </c>
+      <c r="AC13">
+        <v>1</v>
+      </c>
+      <c r="AK13" t="s">
+        <v>24</v>
       </c>
       <c r="AM13" t="s">
-        <v>56</v>
+        <v>46</v>
+      </c>
+      <c r="AN13" t="s">
+        <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C14">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D14">
         <f t="shared" si="1"/>
@@ -2391,12 +2446,9 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="T14">
+      <c r="U14">
         <f t="shared" si="3"/>
-        <v>4</v>
-      </c>
-      <c r="U14">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="V14">
         <v>1</v>
@@ -2407,24 +2459,27 @@
       <c r="X14">
         <v>1</v>
       </c>
-      <c r="AJ14" t="s">
-        <v>15</v>
+      <c r="Y14">
+        <v>1</v>
       </c>
       <c r="AK14" t="s">
-        <v>20</v>
+        <v>14</v>
+      </c>
+      <c r="AL14" t="s">
+        <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C15">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="D15">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E15">
         <v>2</v>
@@ -2450,17 +2505,20 @@
       </c>
       <c r="L15">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="S15">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="M15">
+        <v>1.5</v>
+      </c>
+      <c r="N15">
+        <v>4.5</v>
       </c>
       <c r="T15">
+        <v>1</v>
+      </c>
+      <c r="U15">
         <f t="shared" si="3"/>
-        <v>6</v>
-      </c>
-      <c r="U15">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="V15">
         <v>1</v>
@@ -2477,27 +2535,33 @@
       <c r="Z15">
         <v>1</v>
       </c>
-      <c r="AJ15" t="s">
-        <v>22</v>
-      </c>
-      <c r="AL15" t="s">
-        <v>52</v>
+      <c r="AA15">
+        <v>1</v>
+      </c>
+      <c r="AB15">
+        <v>1</v>
+      </c>
+      <c r="AK15" t="s">
+        <v>21</v>
       </c>
       <c r="AM15" t="s">
-        <v>55</v>
+        <v>51</v>
+      </c>
+      <c r="AN15" t="s">
+        <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C16">
         <f t="shared" si="0"/>
-        <v>15.5</v>
+        <v>34.5</v>
       </c>
       <c r="D16">
         <f t="shared" si="1"/>
-        <v>8.5</v>
+        <v>19.5</v>
       </c>
       <c r="E16">
         <v>2</v>
@@ -2523,17 +2587,23 @@
       </c>
       <c r="L16">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="S16">
-        <v>1</v>
+        <v>11</v>
+      </c>
+      <c r="M16">
+        <v>4</v>
+      </c>
+      <c r="N16">
+        <v>4</v>
+      </c>
+      <c r="O16">
+        <v>3</v>
       </c>
       <c r="T16">
+        <v>1</v>
+      </c>
+      <c r="U16">
         <f t="shared" si="3"/>
-        <v>6</v>
-      </c>
-      <c r="U16">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="V16">
         <v>1</v>
@@ -2550,27 +2620,33 @@
       <c r="Z16">
         <v>1</v>
       </c>
-      <c r="AJ16" t="s">
-        <v>14</v>
-      </c>
-      <c r="AL16" t="s">
-        <v>50</v>
+      <c r="AA16">
+        <v>1</v>
+      </c>
+      <c r="AC16">
+        <v>1</v>
+      </c>
+      <c r="AK16" t="s">
+        <v>13</v>
       </c>
       <c r="AM16" t="s">
-        <v>58</v>
+        <v>49</v>
+      </c>
+      <c r="AN16" t="s">
+        <v>57</v>
       </c>
     </row>
-    <row r="17" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C17">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="D17">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E17">
         <v>1</v>
@@ -2596,14 +2672,20 @@
       </c>
       <c r="L17">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="T17">
+        <v>10</v>
+      </c>
+      <c r="M17">
+        <v>4.5</v>
+      </c>
+      <c r="N17">
+        <v>4</v>
+      </c>
+      <c r="O17">
+        <v>1.5</v>
+      </c>
+      <c r="U17">
         <f t="shared" si="3"/>
-        <v>6</v>
-      </c>
-      <c r="U17">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="V17">
         <v>1</v>
@@ -2620,23 +2702,32 @@
       <c r="Z17">
         <v>1</v>
       </c>
-      <c r="AJ17" t="s">
-        <v>27</v>
+      <c r="AA17">
+        <v>1</v>
+      </c>
+      <c r="AB17">
+        <v>1</v>
+      </c>
+      <c r="AC17">
+        <v>1</v>
       </c>
       <c r="AK17" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="AL17" t="s">
-        <v>59</v>
+        <v>19</v>
+      </c>
+      <c r="AM17" t="s">
+        <v>58</v>
       </c>
     </row>
-    <row r="18" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C18">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="D18">
         <f t="shared" si="1"/>
@@ -2650,12 +2741,9 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="T18">
+      <c r="U18">
         <f t="shared" si="3"/>
-        <v>4</v>
-      </c>
-      <c r="V18">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="W18">
         <v>1</v>
@@ -2666,18 +2754,30 @@
       <c r="Y18">
         <v>1</v>
       </c>
+      <c r="Z18">
+        <v>1</v>
+      </c>
+      <c r="AB18">
+        <v>1</v>
+      </c>
+      <c r="AC18">
+        <v>1</v>
+      </c>
+      <c r="AK18" t="s">
+        <v>66</v>
+      </c>
     </row>
-    <row r="19" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>2</v>
       </c>
       <c r="C19">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="D19">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="E19">
         <v>2</v>
@@ -2703,22 +2803,31 @@
       </c>
       <c r="L19">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="S19">
-        <v>1</v>
+        <v>14</v>
+      </c>
+      <c r="M19">
+        <v>4.5</v>
+      </c>
+      <c r="N19">
+        <v>4.5</v>
+      </c>
+      <c r="O19">
+        <v>3</v>
+      </c>
+      <c r="P19">
+        <v>2</v>
       </c>
       <c r="T19">
+        <v>1</v>
+      </c>
+      <c r="U19">
         <f t="shared" si="3"/>
-        <v>5</v>
-      </c>
-      <c r="U19">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="V19">
         <v>1</v>
       </c>
-      <c r="X19">
+      <c r="W19">
         <v>1</v>
       </c>
       <c r="Y19">
@@ -2727,19 +2836,20 @@
       <c r="Z19">
         <v>1</v>
       </c>
-      <c r="AJ19" t="s">
-        <v>11</v>
-      </c>
-      <c r="AL19" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="21" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="U21" t="s">
-        <v>64</v>
-      </c>
-      <c r="V21" t="s">
-        <v>63</v>
+      <c r="AA19">
+        <v>1</v>
+      </c>
+      <c r="AB19">
+        <v>1</v>
+      </c>
+      <c r="AC19">
+        <v>1</v>
+      </c>
+      <c r="AK19" t="s">
+        <v>10</v>
+      </c>
+      <c r="AM19" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated points for activity and presence, plus info about next class
</commit_message>
<xml_diff>
--- a/Oceny.xlsx
+++ b/Oceny.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="71">
   <si>
     <t>Jablonski Mateusz</t>
   </si>
@@ -231,6 +231,12 @@
   </si>
   <si>
     <t>https://github.com/biedro94</t>
+  </si>
+  <si>
+    <t>Odrabianie zajec: czwartek 4 maja godz 16:00</t>
+  </si>
+  <si>
+    <t>Przypominam, ze jest to ostatni termin zaliczenia zadania z WS.</t>
   </si>
 </sst>
 </file>
@@ -266,8 +272,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -677,13 +684,13 @@
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>8</c:v>
@@ -701,19 +708,19 @@
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>14</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>14</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>16</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>14</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -729,11 +736,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="309333688"/>
-        <c:axId val="309334864"/>
+        <c:axId val="280719480"/>
+        <c:axId val="11224512"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="309333688"/>
+        <c:axId val="280719480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -776,7 +783,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="309334864"/>
+        <c:crossAx val="11224512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -784,7 +791,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="309334864"/>
+        <c:axId val="11224512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -835,7 +842,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="309333688"/>
+        <c:crossAx val="280719480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1759,10 +1766,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:AS19"/>
+  <dimension ref="A4:AS22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="X25" sqref="X25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -2020,7 +2027,7 @@
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D7">
         <f t="shared" si="1"/>
@@ -2066,7 +2073,7 @@
       </c>
       <c r="U7">
         <f t="shared" ref="U7:U19" si="3">SUM(V7:AJ7)*2</f>
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="V7">
         <v>1</v>
@@ -2090,6 +2097,9 @@
         <v>1</v>
       </c>
       <c r="AC7">
+        <v>1</v>
+      </c>
+      <c r="AD7">
         <v>1</v>
       </c>
       <c r="AK7" t="s">
@@ -2154,7 +2164,7 @@
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D9">
         <f t="shared" si="1"/>
@@ -2173,7 +2183,7 @@
       </c>
       <c r="U9">
         <f t="shared" si="3"/>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="W9">
         <v>1</v>
@@ -2191,6 +2201,9 @@
         <v>1</v>
       </c>
       <c r="AC9">
+        <v>1</v>
+      </c>
+      <c r="AD9">
         <v>1</v>
       </c>
       <c r="AK9" t="s">
@@ -2475,7 +2488,7 @@
       </c>
       <c r="C15">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D15">
         <f t="shared" si="1"/>
@@ -2518,7 +2531,7 @@
       </c>
       <c r="U15">
         <f t="shared" si="3"/>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="V15">
         <v>1</v>
@@ -2539,6 +2552,9 @@
         <v>1</v>
       </c>
       <c r="AB15">
+        <v>1</v>
+      </c>
+      <c r="AD15">
         <v>1</v>
       </c>
       <c r="AK15" t="s">
@@ -2557,7 +2573,7 @@
       </c>
       <c r="C16">
         <f t="shared" si="0"/>
-        <v>34.5</v>
+        <v>36.5</v>
       </c>
       <c r="D16">
         <f t="shared" si="1"/>
@@ -2603,7 +2619,7 @@
       </c>
       <c r="U16">
         <f t="shared" si="3"/>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="V16">
         <v>1</v>
@@ -2624,6 +2640,9 @@
         <v>1</v>
       </c>
       <c r="AC16">
+        <v>1</v>
+      </c>
+      <c r="AD16">
         <v>1</v>
       </c>
       <c r="AK16" t="s">
@@ -2642,7 +2661,7 @@
       </c>
       <c r="C17">
         <f t="shared" si="0"/>
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D17">
         <f t="shared" si="1"/>
@@ -2685,7 +2704,7 @@
       </c>
       <c r="U17">
         <f t="shared" si="3"/>
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="V17">
         <v>1</v>
@@ -2709,6 +2728,9 @@
         <v>1</v>
       </c>
       <c r="AC17">
+        <v>1</v>
+      </c>
+      <c r="AD17">
         <v>1</v>
       </c>
       <c r="AK17" t="s">
@@ -2773,7 +2795,7 @@
       </c>
       <c r="C19">
         <f t="shared" si="0"/>
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D19">
         <f t="shared" si="1"/>
@@ -2822,7 +2844,7 @@
       </c>
       <c r="U19">
         <f t="shared" si="3"/>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="V19">
         <v>1</v>
@@ -2843,6 +2865,9 @@
         <v>1</v>
       </c>
       <c r="AC19">
+        <v>1</v>
+      </c>
+      <c r="AD19">
         <v>1</v>
       </c>
       <c r="AK19" t="s">
@@ -2851,6 +2876,17 @@
       <c r="AM19" t="s">
         <v>48</v>
       </c>
+    </row>
+    <row r="21" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="W21" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="W22" t="s">
+        <v>70</v>
+      </c>
+      <c r="X22" s="1"/>
     </row>
   </sheetData>
   <sortState ref="A6:M19">

</xml_diff>

<commit_message>
updated scoring for ws
</commit_message>
<xml_diff>
--- a/Oceny.xlsx
+++ b/Oceny.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="77">
   <si>
     <t>Jablonski Mateusz</t>
   </si>
@@ -233,10 +233,28 @@
     <t>https://github.com/biedro94</t>
   </si>
   <si>
-    <t>Odrabianie zajec: czwartek 4 maja godz 16:00</t>
-  </si>
-  <si>
-    <t>Przypominam, ze jest to ostatni termin zaliczenia zadania z WS.</t>
+    <t>rest client</t>
+  </si>
+  <si>
+    <t>rest serv</t>
+  </si>
+  <si>
+    <t>soap</t>
+  </si>
+  <si>
+    <t>Przecchodzi 7/14 testow</t>
+  </si>
+  <si>
+    <t>formatter, zbedne komentarze TODO</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Niezle nazwane commity. Testy, nazewnictwo, poprawnosc restclient.</t>
+  </si>
+  <si>
+    <t>testy nie przechodza wszystkie, ale bylo blisko</t>
+  </si>
+  <si>
+    <t>4?</t>
   </si>
 </sst>
 </file>
@@ -453,7 +471,7 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16</c:v>
+                  <c:v>29.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>2</c:v>
@@ -462,7 +480,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>3</c:v>
@@ -483,13 +501,13 @@
                   <c:v>19.5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>20</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>23</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -500,7 +518,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$T$5</c:f>
+              <c:f>Sheet1!$W$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -571,7 +589,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$T$6:$T$19</c:f>
+              <c:f>Sheet1!$W$6:$W$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
@@ -593,8 +611,11 @@
                 <c:pt idx="10">
                   <c:v>1</c:v>
                 </c:pt>
+                <c:pt idx="11">
+                  <c:v>2</c:v>
+                </c:pt>
                 <c:pt idx="13">
-                  <c:v>1</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -605,7 +626,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$U$5</c:f>
+              <c:f>Sheet1!$X$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -676,7 +697,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$U$6:$U$19</c:f>
+              <c:f>Sheet1!$X$6:$X$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
@@ -684,7 +705,7 @@
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>8</c:v>
@@ -693,7 +714,7 @@
                   <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>12</c:v>
@@ -702,7 +723,7 @@
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>16</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>8</c:v>
@@ -714,13 +735,13 @@
                   <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>16</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -736,11 +757,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="280719480"/>
-        <c:axId val="11224512"/>
+        <c:axId val="269195672"/>
+        <c:axId val="269194496"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="280719480"/>
+        <c:axId val="269195672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -783,7 +804,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="11224512"/>
+        <c:crossAx val="269194496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -791,7 +812,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="11224512"/>
+        <c:axId val="269194496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -842,7 +863,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="280719480"/>
+        <c:crossAx val="269195672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1478,7 +1499,7 @@
       <xdr:rowOff>14286</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
+      <xdr:col>23</xdr:col>
       <xdr:colOff>581025</xdr:colOff>
       <xdr:row>35</xdr:row>
       <xdr:rowOff>38099</xdr:rowOff>
@@ -1766,10 +1787,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:AS22"/>
+  <dimension ref="A4:AV22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="X25" sqref="X25"/>
+      <selection activeCell="S17" sqref="S17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -1784,64 +1805,65 @@
     <col min="12" max="12" width="9.140625" customWidth="1" collapsed="1"/>
     <col min="13" max="16" width="9.140625" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="17" max="17" width="9.140625" collapsed="1"/>
-    <col min="18" max="18" width="9.85546875" customWidth="1"/>
-    <col min="19" max="19" width="11.7109375" customWidth="1"/>
-    <col min="22" max="35" width="9.140625" customWidth="1" outlineLevel="1"/>
-    <col min="36" max="36" width="9.5703125" customWidth="1" outlineLevel="1"/>
-    <col min="37" max="37" width="35.5703125" customWidth="1"/>
-    <col min="38" max="39" width="17.5703125" customWidth="1"/>
-    <col min="40" max="41" width="16.42578125" customWidth="1"/>
-    <col min="42" max="42" width="16.7109375" customWidth="1"/>
+    <col min="18" max="20" width="9.140625" customWidth="1" outlineLevel="1"/>
+    <col min="21" max="21" width="9.85546875" customWidth="1"/>
+    <col min="22" max="22" width="11.7109375" customWidth="1"/>
+    <col min="25" max="38" width="9.140625" customWidth="1" outlineLevel="1"/>
+    <col min="39" max="39" width="9.5703125" customWidth="1" outlineLevel="1"/>
+    <col min="40" max="40" width="35.5703125" customWidth="1"/>
+    <col min="41" max="42" width="17.5703125" customWidth="1"/>
+    <col min="43" max="44" width="16.42578125" customWidth="1"/>
+    <col min="45" max="45" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="V4">
-        <v>1</v>
-      </c>
-      <c r="W4">
+    <row r="4" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="Y4">
+        <v>1</v>
+      </c>
+      <c r="Z4">
         <v>2</v>
       </c>
-      <c r="X4">
+      <c r="AA4">
         <v>3</v>
       </c>
-      <c r="Y4">
+      <c r="AB4">
         <v>4</v>
       </c>
-      <c r="Z4">
+      <c r="AC4">
         <v>5</v>
       </c>
-      <c r="AA4">
+      <c r="AD4">
         <v>6</v>
       </c>
-      <c r="AB4">
+      <c r="AE4">
         <v>7</v>
       </c>
-      <c r="AC4">
+      <c r="AF4">
         <v>8</v>
       </c>
-      <c r="AD4">
+      <c r="AG4">
         <v>9</v>
       </c>
-      <c r="AE4">
+      <c r="AH4">
         <v>10</v>
       </c>
-      <c r="AF4">
+      <c r="AI4">
         <v>11</v>
       </c>
-      <c r="AG4">
+      <c r="AJ4">
         <v>12</v>
       </c>
-      <c r="AH4">
+      <c r="AK4">
         <v>13</v>
       </c>
-      <c r="AI4">
+      <c r="AL4">
         <v>14</v>
       </c>
-      <c r="AJ4">
+      <c r="AM4">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>60</v>
       </c>
@@ -1894,100 +1916,109 @@
         <v>29</v>
       </c>
       <c r="R5" t="s">
+        <v>69</v>
+      </c>
+      <c r="S5" t="s">
+        <v>70</v>
+      </c>
+      <c r="T5" t="s">
+        <v>71</v>
+      </c>
+      <c r="U5" t="s">
         <v>6</v>
       </c>
-      <c r="S5" t="s">
+      <c r="V5" t="s">
         <v>7</v>
       </c>
-      <c r="T5" t="s">
+      <c r="W5" t="s">
         <v>61</v>
       </c>
-      <c r="U5" t="s">
+      <c r="X5" t="s">
         <v>44</v>
       </c>
-      <c r="V5">
+      <c r="Y5">
         <v>22.02</v>
       </c>
-      <c r="W5">
+      <c r="Z5">
         <v>1.03</v>
       </c>
-      <c r="X5">
+      <c r="AA5">
         <v>15.03</v>
       </c>
-      <c r="Y5">
+      <c r="AB5">
         <v>22.03</v>
       </c>
-      <c r="Z5">
+      <c r="AC5">
         <v>29.03</v>
       </c>
-      <c r="AA5">
+      <c r="AD5">
         <v>5.04</v>
       </c>
-      <c r="AB5">
+      <c r="AE5">
         <v>12.04</v>
       </c>
-      <c r="AC5">
+      <c r="AF5">
         <v>19.04</v>
       </c>
-      <c r="AD5">
+      <c r="AG5">
         <v>26.04</v>
       </c>
-      <c r="AE5">
-        <v>3.05</v>
-      </c>
-      <c r="AF5">
+      <c r="AH5">
+        <v>4.05</v>
+      </c>
+      <c r="AI5">
         <v>10.050000000000001</v>
       </c>
-      <c r="AG5">
+      <c r="AJ5">
         <v>17.05</v>
       </c>
-      <c r="AH5">
+      <c r="AK5">
         <v>24.05</v>
       </c>
-      <c r="AI5">
+      <c r="AL5">
         <v>31.05</v>
       </c>
-      <c r="AJ5">
+      <c r="AM5">
         <v>7.06</v>
       </c>
-      <c r="AK5" t="s">
+      <c r="AN5" t="s">
         <v>9</v>
       </c>
-      <c r="AL5" t="s">
+      <c r="AO5" t="s">
         <v>45</v>
       </c>
-      <c r="AM5" t="s">
+      <c r="AP5" t="s">
         <v>50</v>
       </c>
-      <c r="AN5" t="s">
+      <c r="AQ5" t="s">
         <v>52</v>
       </c>
-      <c r="AO5" t="s">
+      <c r="AR5" t="s">
         <v>53</v>
       </c>
-      <c r="AP5" t="s">
+      <c r="AS5" t="s">
         <v>15</v>
       </c>
-      <c r="AQ5" t="s">
+      <c r="AT5" t="s">
         <v>16</v>
       </c>
-      <c r="AR5" t="s">
+      <c r="AU5" t="s">
         <v>17</v>
       </c>
-      <c r="AS5" t="s">
+      <c r="AV5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>38</v>
       </c>
       <c r="C6">
-        <f t="shared" ref="C6:C19" si="0">D6+U6+T6</f>
+        <f>D6+X6+W6</f>
         <v>10</v>
       </c>
       <c r="D6">
-        <f t="shared" ref="D6:D19" si="1">SUM(E6,F6,L6,Q6,R6,S6)</f>
+        <f>SUM(E6,F6,L6,Q6,U6,V6)</f>
         <v>2</v>
       </c>
       <c r="E6">
@@ -2001,37 +2032,41 @@
         <f>SUM(M6:P6)</f>
         <v>0</v>
       </c>
-      <c r="U6">
-        <f>SUM(V6:AJ6)*2</f>
+      <c r="Q6">
+        <f>SUM(R6:T6)</f>
+        <v>0</v>
+      </c>
+      <c r="X6">
+        <f>SUM(Y6:AM6)*2</f>
         <v>8</v>
       </c>
-      <c r="V6">
-        <v>1</v>
-      </c>
-      <c r="W6">
-        <v>1</v>
-      </c>
-      <c r="X6">
-        <v>1</v>
-      </c>
       <c r="Y6">
         <v>1</v>
       </c>
-      <c r="AK6" t="s">
+      <c r="Z6">
+        <v>1</v>
+      </c>
+      <c r="AA6">
+        <v>1</v>
+      </c>
+      <c r="AB6">
+        <v>1</v>
+      </c>
+      <c r="AN6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>37</v>
       </c>
       <c r="C7">
-        <f t="shared" si="0"/>
-        <v>35</v>
+        <f>D7+X7+W7</f>
+        <v>50.5</v>
       </c>
       <c r="D7">
-        <f t="shared" si="1"/>
-        <v>16</v>
+        <f>SUM(E7,F7,L7,Q7,U7,V7)</f>
+        <v>29.5</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -2056,7 +2091,7 @@
         <v>0</v>
       </c>
       <c r="L7">
-        <f t="shared" ref="L7:L19" si="2">SUM(M7:P7)</f>
+        <f t="shared" ref="L7:L19" si="0">SUM(M7:P7)</f>
         <v>9.5</v>
       </c>
       <c r="M7">
@@ -2068,21 +2103,25 @@
       <c r="O7">
         <v>1.5</v>
       </c>
+      <c r="Q7">
+        <f t="shared" ref="Q7:Q19" si="1">SUM(R7:T7)</f>
+        <v>13.5</v>
+      </c>
+      <c r="R7">
+        <v>3.5</v>
+      </c>
+      <c r="S7">
+        <v>5</v>
+      </c>
       <c r="T7">
-        <v>1</v>
-      </c>
-      <c r="U7">
-        <f t="shared" ref="U7:U19" si="3">SUM(V7:AJ7)*2</f>
-        <v>18</v>
-      </c>
-      <c r="V7">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="W7">
         <v>1</v>
       </c>
       <c r="X7">
-        <v>1</v>
+        <f t="shared" ref="X7:X19" si="2">SUM(Y7:AM7)*2</f>
+        <v>20</v>
       </c>
       <c r="Y7">
         <v>1</v>
@@ -2102,710 +2141,856 @@
       <c r="AD7">
         <v>1</v>
       </c>
-      <c r="AK7" t="s">
+      <c r="AE7">
+        <v>1</v>
+      </c>
+      <c r="AF7">
+        <v>1</v>
+      </c>
+      <c r="AG7">
+        <v>1</v>
+      </c>
+      <c r="AH7">
+        <v>1</v>
+      </c>
+      <c r="AN7" t="s">
         <v>27</v>
       </c>
-      <c r="AL7" t="s">
+      <c r="AO7" t="s">
         <v>19</v>
       </c>
-      <c r="AM7" t="s">
+      <c r="AP7" t="s">
         <v>47</v>
       </c>
-      <c r="AN7" t="s">
+      <c r="AQ7" t="s">
         <v>56</v>
       </c>
+      <c r="AT7" t="s">
+        <v>74</v>
+      </c>
     </row>
-    <row r="8" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>36</v>
       </c>
       <c r="C8">
+        <f>D8+X8+W8</f>
+        <v>10</v>
+      </c>
+      <c r="D8">
+        <f>SUM(E8,F8,L8,Q8,U8,V8)</f>
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8">
+        <f t="shared" ref="F8:F19" si="3">SUM(G8:K8)</f>
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="X8">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="Y8">
+        <v>1</v>
+      </c>
+      <c r="Z8">
+        <v>1</v>
+      </c>
+      <c r="AA8">
+        <v>1</v>
+      </c>
+      <c r="AB8">
+        <v>1</v>
+      </c>
+      <c r="AN8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <f>D9+X9+W9</f>
+        <v>15</v>
+      </c>
+      <c r="D9">
+        <f>SUM(E9,F9,L9,Q9,U9,V9)</f>
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="W9">
+        <v>1</v>
+      </c>
+      <c r="X9">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="Z9">
+        <v>1</v>
+      </c>
+      <c r="AA9">
+        <v>1</v>
+      </c>
+      <c r="AB9">
+        <v>1</v>
+      </c>
+      <c r="AC9">
+        <v>1</v>
+      </c>
+      <c r="AE9">
+        <v>1</v>
+      </c>
+      <c r="AF9">
+        <v>1</v>
+      </c>
+      <c r="AG9">
+        <v>1</v>
+      </c>
+      <c r="AN9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10">
+        <f>D10+X10+W10</f>
+        <v>13.5</v>
+      </c>
+      <c r="D10">
+        <f>SUM(E10,F10,L10,Q10,U10,V10)</f>
+        <v>2.5</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" si="1"/>
+        <v>2.5</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="S10">
+        <v>2.5</v>
+      </c>
+      <c r="T10">
+        <v>0</v>
+      </c>
+      <c r="W10">
+        <v>1</v>
+      </c>
+      <c r="X10">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="Z10">
+        <v>1</v>
+      </c>
+      <c r="AA10">
+        <v>1</v>
+      </c>
+      <c r="AC10">
+        <v>1</v>
+      </c>
+      <c r="AD10">
+        <v>1</v>
+      </c>
+      <c r="AH10">
+        <v>1</v>
+      </c>
+      <c r="AN10" t="s">
+        <v>68</v>
+      </c>
+      <c r="AT10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <f>D11+X11+W11</f>
+        <v>15</v>
+      </c>
+      <c r="D11">
+        <f>SUM(E11,F11,L11,Q11,U11,V11)</f>
+        <v>3</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <v>0</v>
+      </c>
+      <c r="S11">
+        <v>0</v>
+      </c>
+      <c r="T11">
+        <v>0</v>
+      </c>
+      <c r="X11">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="Y11">
+        <v>1</v>
+      </c>
+      <c r="Z11">
+        <v>1</v>
+      </c>
+      <c r="AA11">
+        <v>1</v>
+      </c>
+      <c r="AC11">
+        <v>1</v>
+      </c>
+      <c r="AD11">
+        <v>1</v>
+      </c>
+      <c r="AE11">
+        <v>1</v>
+      </c>
+      <c r="AN11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12">
+        <f>D12+X12+W12</f>
+        <v>6</v>
+      </c>
+      <c r="D12">
+        <f>SUM(E12,F12,L12,Q12,U12,V12)</f>
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="X12">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="Z12">
+        <v>1</v>
+      </c>
+      <c r="AA12">
+        <v>1</v>
+      </c>
+      <c r="AB12">
+        <v>1</v>
+      </c>
+      <c r="AN12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13">
+        <f>D13+X13+W13</f>
+        <v>43.5</v>
+      </c>
+      <c r="D13">
+        <f>SUM(E13,F13,L13,Q13,U13,V13)</f>
+        <v>24.5</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="3"/>
+        <v>8.5</v>
+      </c>
+      <c r="G13">
+        <v>2</v>
+      </c>
+      <c r="H13">
+        <v>2</v>
+      </c>
+      <c r="I13">
+        <v>2</v>
+      </c>
+      <c r="J13">
+        <v>1.5</v>
+      </c>
+      <c r="K13">
+        <v>1</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="M13">
+        <v>4.5</v>
+      </c>
+      <c r="N13">
+        <v>4.5</v>
+      </c>
+      <c r="O13">
+        <v>3</v>
+      </c>
+      <c r="P13">
+        <v>2</v>
+      </c>
+      <c r="Q13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R13">
+        <v>0</v>
+      </c>
+      <c r="S13">
+        <v>0</v>
+      </c>
+      <c r="T13">
+        <v>0</v>
+      </c>
+      <c r="W13">
+        <v>1</v>
+      </c>
+      <c r="X13">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="Y13">
+        <v>1</v>
+      </c>
+      <c r="Z13">
+        <v>1</v>
+      </c>
+      <c r="AA13">
+        <v>1</v>
+      </c>
+      <c r="AB13">
+        <v>1</v>
+      </c>
+      <c r="AC13">
+        <v>1</v>
+      </c>
+      <c r="AD13">
+        <v>1</v>
+      </c>
+      <c r="AE13">
+        <v>1</v>
+      </c>
+      <c r="AF13">
+        <v>1</v>
+      </c>
+      <c r="AH13">
+        <v>1</v>
+      </c>
+      <c r="AN13" t="s">
+        <v>24</v>
+      </c>
+      <c r="AP13" t="s">
+        <v>46</v>
+      </c>
+      <c r="AQ13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14">
+        <f>D14+X14+W14</f>
+        <v>9</v>
+      </c>
+      <c r="D14">
+        <f>SUM(E14,F14,L14,Q14,U14,V14)</f>
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="X14">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="Y14">
+        <v>1</v>
+      </c>
+      <c r="Z14">
+        <v>1</v>
+      </c>
+      <c r="AA14">
+        <v>1</v>
+      </c>
+      <c r="AB14">
+        <v>1</v>
+      </c>
+      <c r="AN14" t="s">
+        <v>14</v>
+      </c>
+      <c r="AO14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15">
+        <f>D15+X15+W15</f>
+        <v>32</v>
+      </c>
+      <c r="D15">
+        <f>SUM(E15,F15,L15,Q15,U15,V15)</f>
+        <v>15</v>
+      </c>
+      <c r="E15">
+        <v>2</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="G15">
+        <v>2</v>
+      </c>
+      <c r="H15">
+        <v>2</v>
+      </c>
+      <c r="I15">
+        <v>2</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>1</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="M15">
+        <v>1.5</v>
+      </c>
+      <c r="N15">
+        <v>4.5</v>
+      </c>
+      <c r="Q15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R15">
+        <v>0</v>
+      </c>
+      <c r="S15">
+        <v>0</v>
+      </c>
+      <c r="T15">
+        <v>0</v>
+      </c>
+      <c r="W15">
+        <v>1</v>
+      </c>
+      <c r="X15">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="Y15">
+        <v>1</v>
+      </c>
+      <c r="Z15">
+        <v>1</v>
+      </c>
+      <c r="AA15">
+        <v>1</v>
+      </c>
+      <c r="AB15">
+        <v>1</v>
+      </c>
+      <c r="AC15">
+        <v>1</v>
+      </c>
+      <c r="AD15">
+        <v>1</v>
+      </c>
+      <c r="AE15">
+        <v>1</v>
+      </c>
+      <c r="AG15">
+        <v>1</v>
+      </c>
+      <c r="AN15" t="s">
+        <v>21</v>
+      </c>
+      <c r="AP15" t="s">
+        <v>51</v>
+      </c>
+      <c r="AQ15" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16">
+        <f>D16+X16+W16</f>
+        <v>36.5</v>
+      </c>
+      <c r="D16">
+        <f>SUM(E16,F16,L16,Q16,U16,V16)</f>
+        <v>19.5</v>
+      </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="3"/>
+        <v>6.5</v>
+      </c>
+      <c r="G16">
+        <v>2</v>
+      </c>
+      <c r="H16">
+        <v>2</v>
+      </c>
+      <c r="I16">
+        <v>1</v>
+      </c>
+      <c r="J16">
+        <v>0.5</v>
+      </c>
+      <c r="K16">
+        <v>1</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="M16">
+        <v>4</v>
+      </c>
+      <c r="N16">
+        <v>4</v>
+      </c>
+      <c r="O16">
+        <v>3</v>
+      </c>
+      <c r="Q16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R16" t="s">
+        <v>76</v>
+      </c>
+      <c r="S16" t="s">
+        <v>76</v>
+      </c>
+      <c r="T16">
+        <v>0</v>
+      </c>
+      <c r="W16">
+        <v>1</v>
+      </c>
+      <c r="X16">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="Y16">
+        <v>1</v>
+      </c>
+      <c r="Z16">
+        <v>1</v>
+      </c>
+      <c r="AA16">
+        <v>1</v>
+      </c>
+      <c r="AB16">
+        <v>1</v>
+      </c>
+      <c r="AC16">
+        <v>1</v>
+      </c>
+      <c r="AD16">
+        <v>1</v>
+      </c>
+      <c r="AF16">
+        <v>1</v>
+      </c>
+      <c r="AG16">
+        <v>1</v>
+      </c>
+      <c r="AN16" t="s">
+        <v>13</v>
+      </c>
+      <c r="AP16" t="s">
+        <v>49</v>
+      </c>
+      <c r="AQ16" t="s">
+        <v>57</v>
+      </c>
+      <c r="AT16" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17">
+        <f>D17+X17+W17</f>
+        <v>55</v>
+      </c>
+      <c r="D17">
+        <f>SUM(E17,F17,L17,Q17,U17,V17)</f>
+        <v>33</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="G17">
+        <v>2</v>
+      </c>
+      <c r="H17">
+        <v>2</v>
+      </c>
+      <c r="I17">
+        <v>1.5</v>
+      </c>
+      <c r="J17">
+        <v>2</v>
+      </c>
+      <c r="K17">
+        <v>1.5</v>
+      </c>
+      <c r="L17">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="D8">
+      <c r="M17">
+        <v>4.5</v>
+      </c>
+      <c r="N17">
+        <v>4</v>
+      </c>
+      <c r="O17">
+        <v>1.5</v>
+      </c>
+      <c r="Q17">
         <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="R17">
+        <v>4</v>
+      </c>
+      <c r="S17">
+        <v>5</v>
+      </c>
+      <c r="T17">
+        <v>4</v>
+      </c>
+      <c r="W17">
         <v>2</v>
       </c>
-      <c r="E8">
-        <v>2</v>
-      </c>
-      <c r="F8">
-        <f t="shared" ref="F8:F19" si="4">SUM(G8:K8)</f>
-        <v>0</v>
-      </c>
-      <c r="L8">
+      <c r="X17">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="U8">
+        <v>20</v>
+      </c>
+      <c r="Y17">
+        <v>1</v>
+      </c>
+      <c r="Z17">
+        <v>1</v>
+      </c>
+      <c r="AA17">
+        <v>1</v>
+      </c>
+      <c r="AB17">
+        <v>1</v>
+      </c>
+      <c r="AC17">
+        <v>1</v>
+      </c>
+      <c r="AD17">
+        <v>1</v>
+      </c>
+      <c r="AE17">
+        <v>1</v>
+      </c>
+      <c r="AF17">
+        <v>1</v>
+      </c>
+      <c r="AG17">
+        <v>1</v>
+      </c>
+      <c r="AH17">
+        <v>1</v>
+      </c>
+      <c r="AN17" t="s">
+        <v>26</v>
+      </c>
+      <c r="AO17" t="s">
+        <v>19</v>
+      </c>
+      <c r="AP17" t="s">
+        <v>58</v>
+      </c>
+      <c r="AT17" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18">
+        <f>D18+X18+W18</f>
+        <v>16.5</v>
+      </c>
+      <c r="D18">
+        <f>SUM(E18,F18,L18,Q18,U18,V18)</f>
+        <v>2.5</v>
+      </c>
+      <c r="F18">
         <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="V8">
-        <v>1</v>
-      </c>
-      <c r="W8">
-        <v>1</v>
-      </c>
-      <c r="X8">
-        <v>1</v>
-      </c>
-      <c r="Y8">
-        <v>1</v>
-      </c>
-      <c r="AK8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="L18">
         <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="Q18">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="L9">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="T9">
-        <v>1</v>
-      </c>
-      <c r="U9">
-        <f t="shared" si="3"/>
-        <v>14</v>
-      </c>
-      <c r="W9">
-        <v>1</v>
-      </c>
-      <c r="X9">
-        <v>1</v>
-      </c>
-      <c r="Y9">
-        <v>1</v>
-      </c>
-      <c r="Z9">
-        <v>1</v>
-      </c>
-      <c r="AB9">
-        <v>1</v>
-      </c>
-      <c r="AC9">
-        <v>1</v>
-      </c>
-      <c r="AD9">
-        <v>1</v>
-      </c>
-      <c r="AK9" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="10" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="D10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="L10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="T10">
-        <v>1</v>
-      </c>
-      <c r="U10">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="W10">
-        <v>1</v>
-      </c>
-      <c r="X10">
-        <v>1</v>
-      </c>
-      <c r="Z10">
-        <v>1</v>
-      </c>
-      <c r="AA10">
-        <v>1</v>
-      </c>
-      <c r="AK10" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="11" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C11">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="D11">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="E11">
-        <v>2</v>
-      </c>
-      <c r="F11">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="G11">
-        <v>1</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="L11">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="U11">
-        <f t="shared" si="3"/>
-        <v>12</v>
-      </c>
-      <c r="V11">
-        <v>1</v>
-      </c>
-      <c r="W11">
-        <v>1</v>
-      </c>
-      <c r="X11">
-        <v>1</v>
-      </c>
-      <c r="Z11">
-        <v>1</v>
-      </c>
-      <c r="AA11">
-        <v>1</v>
-      </c>
-      <c r="AB11">
-        <v>1</v>
-      </c>
-      <c r="AK11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="D12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F12">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="L12">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="U12">
-        <f t="shared" si="3"/>
-        <v>6</v>
-      </c>
-      <c r="W12">
-        <v>1</v>
-      </c>
-      <c r="X12">
-        <v>1</v>
-      </c>
-      <c r="Y12">
-        <v>1</v>
-      </c>
-      <c r="AK12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>34</v>
-      </c>
-      <c r="C13">
-        <f t="shared" si="0"/>
-        <v>41.5</v>
-      </c>
-      <c r="D13">
-        <f t="shared" si="1"/>
-        <v>24.5</v>
-      </c>
-      <c r="E13">
-        <v>2</v>
-      </c>
-      <c r="F13">
-        <f t="shared" si="4"/>
-        <v>8.5</v>
-      </c>
-      <c r="G13">
-        <v>2</v>
-      </c>
-      <c r="H13">
-        <v>2</v>
-      </c>
-      <c r="I13">
-        <v>2</v>
-      </c>
-      <c r="J13">
-        <v>1.5</v>
-      </c>
-      <c r="K13">
-        <v>1</v>
-      </c>
-      <c r="L13">
+        <v>2.5</v>
+      </c>
+      <c r="R18">
+        <v>0</v>
+      </c>
+      <c r="S18">
+        <v>2.5</v>
+      </c>
+      <c r="T18">
+        <v>0</v>
+      </c>
+      <c r="X18">
         <f t="shared" si="2"/>
         <v>14</v>
       </c>
-      <c r="M13">
-        <v>4.5</v>
-      </c>
-      <c r="N13">
-        <v>4.5</v>
-      </c>
-      <c r="O13">
-        <v>3</v>
-      </c>
-      <c r="P13">
-        <v>2</v>
-      </c>
-      <c r="T13">
-        <v>1</v>
-      </c>
-      <c r="U13">
-        <f t="shared" si="3"/>
-        <v>16</v>
-      </c>
-      <c r="V13">
-        <v>1</v>
-      </c>
-      <c r="W13">
-        <v>1</v>
-      </c>
-      <c r="X13">
-        <v>1</v>
-      </c>
-      <c r="Y13">
-        <v>1</v>
-      </c>
-      <c r="Z13">
-        <v>1</v>
-      </c>
-      <c r="AA13">
-        <v>1</v>
-      </c>
-      <c r="AB13">
-        <v>1</v>
-      </c>
-      <c r="AC13">
-        <v>1</v>
-      </c>
-      <c r="AK13" t="s">
-        <v>24</v>
-      </c>
-      <c r="AM13" t="s">
-        <v>46</v>
-      </c>
-      <c r="AN13" t="s">
-        <v>55</v>
+      <c r="Z18">
+        <v>1</v>
+      </c>
+      <c r="AA18">
+        <v>1</v>
+      </c>
+      <c r="AB18">
+        <v>1</v>
+      </c>
+      <c r="AC18">
+        <v>1</v>
+      </c>
+      <c r="AE18">
+        <v>1</v>
+      </c>
+      <c r="AF18">
+        <v>1</v>
+      </c>
+      <c r="AH18">
+        <v>1</v>
+      </c>
+      <c r="AN18" t="s">
+        <v>66</v>
       </c>
     </row>
-    <row r="14" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="D14">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="E14">
-        <v>1</v>
-      </c>
-      <c r="F14">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="L14">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="U14">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="V14">
-        <v>1</v>
-      </c>
-      <c r="W14">
-        <v>1</v>
-      </c>
-      <c r="X14">
-        <v>1</v>
-      </c>
-      <c r="Y14">
-        <v>1</v>
-      </c>
-      <c r="AK14" t="s">
-        <v>14</v>
-      </c>
-      <c r="AL14" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>32</v>
-      </c>
-      <c r="C15">
-        <f t="shared" si="0"/>
-        <v>32</v>
-      </c>
-      <c r="D15">
-        <f t="shared" si="1"/>
-        <v>15</v>
-      </c>
-      <c r="E15">
-        <v>2</v>
-      </c>
-      <c r="F15">
-        <f t="shared" si="4"/>
-        <v>7</v>
-      </c>
-      <c r="G15">
-        <v>2</v>
-      </c>
-      <c r="H15">
-        <v>2</v>
-      </c>
-      <c r="I15">
-        <v>2</v>
-      </c>
-      <c r="J15">
-        <v>0</v>
-      </c>
-      <c r="K15">
-        <v>1</v>
-      </c>
-      <c r="L15">
-        <f t="shared" si="2"/>
-        <v>6</v>
-      </c>
-      <c r="M15">
-        <v>1.5</v>
-      </c>
-      <c r="N15">
-        <v>4.5</v>
-      </c>
-      <c r="T15">
-        <v>1</v>
-      </c>
-      <c r="U15">
-        <f t="shared" si="3"/>
-        <v>16</v>
-      </c>
-      <c r="V15">
-        <v>1</v>
-      </c>
-      <c r="W15">
-        <v>1</v>
-      </c>
-      <c r="X15">
-        <v>1</v>
-      </c>
-      <c r="Y15">
-        <v>1</v>
-      </c>
-      <c r="Z15">
-        <v>1</v>
-      </c>
-      <c r="AA15">
-        <v>1</v>
-      </c>
-      <c r="AB15">
-        <v>1</v>
-      </c>
-      <c r="AD15">
-        <v>1</v>
-      </c>
-      <c r="AK15" t="s">
-        <v>21</v>
-      </c>
-      <c r="AM15" t="s">
-        <v>51</v>
-      </c>
-      <c r="AN15" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="16" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>31</v>
-      </c>
-      <c r="C16">
-        <f t="shared" si="0"/>
-        <v>36.5</v>
-      </c>
-      <c r="D16">
-        <f t="shared" si="1"/>
-        <v>19.5</v>
-      </c>
-      <c r="E16">
-        <v>2</v>
-      </c>
-      <c r="F16">
-        <f t="shared" si="4"/>
-        <v>6.5</v>
-      </c>
-      <c r="G16">
-        <v>2</v>
-      </c>
-      <c r="H16">
-        <v>2</v>
-      </c>
-      <c r="I16">
-        <v>1</v>
-      </c>
-      <c r="J16">
-        <v>0.5</v>
-      </c>
-      <c r="K16">
-        <v>1</v>
-      </c>
-      <c r="L16">
-        <f t="shared" si="2"/>
-        <v>11</v>
-      </c>
-      <c r="M16">
-        <v>4</v>
-      </c>
-      <c r="N16">
-        <v>4</v>
-      </c>
-      <c r="O16">
-        <v>3</v>
-      </c>
-      <c r="T16">
-        <v>1</v>
-      </c>
-      <c r="U16">
-        <f t="shared" si="3"/>
-        <v>16</v>
-      </c>
-      <c r="V16">
-        <v>1</v>
-      </c>
-      <c r="W16">
-        <v>1</v>
-      </c>
-      <c r="X16">
-        <v>1</v>
-      </c>
-      <c r="Y16">
-        <v>1</v>
-      </c>
-      <c r="Z16">
-        <v>1</v>
-      </c>
-      <c r="AA16">
-        <v>1</v>
-      </c>
-      <c r="AC16">
-        <v>1</v>
-      </c>
-      <c r="AD16">
-        <v>1</v>
-      </c>
-      <c r="AK16" t="s">
-        <v>13</v>
-      </c>
-      <c r="AM16" t="s">
-        <v>49</v>
-      </c>
-      <c r="AN16" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="17" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>30</v>
-      </c>
-      <c r="C17">
-        <f t="shared" si="0"/>
-        <v>38</v>
-      </c>
-      <c r="D17">
-        <f t="shared" si="1"/>
-        <v>20</v>
-      </c>
-      <c r="E17">
-        <v>1</v>
-      </c>
-      <c r="F17">
-        <f t="shared" si="4"/>
-        <v>9</v>
-      </c>
-      <c r="G17">
-        <v>2</v>
-      </c>
-      <c r="H17">
-        <v>2</v>
-      </c>
-      <c r="I17">
-        <v>1.5</v>
-      </c>
-      <c r="J17">
-        <v>2</v>
-      </c>
-      <c r="K17">
-        <v>1.5</v>
-      </c>
-      <c r="L17">
-        <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-      <c r="M17">
-        <v>4.5</v>
-      </c>
-      <c r="N17">
-        <v>4</v>
-      </c>
-      <c r="O17">
-        <v>1.5</v>
-      </c>
-      <c r="U17">
-        <f t="shared" si="3"/>
-        <v>18</v>
-      </c>
-      <c r="V17">
-        <v>1</v>
-      </c>
-      <c r="W17">
-        <v>1</v>
-      </c>
-      <c r="X17">
-        <v>1</v>
-      </c>
-      <c r="Y17">
-        <v>1</v>
-      </c>
-      <c r="Z17">
-        <v>1</v>
-      </c>
-      <c r="AA17">
-        <v>1</v>
-      </c>
-      <c r="AB17">
-        <v>1</v>
-      </c>
-      <c r="AC17">
-        <v>1</v>
-      </c>
-      <c r="AD17">
-        <v>1</v>
-      </c>
-      <c r="AK17" t="s">
-        <v>26</v>
-      </c>
-      <c r="AL17" t="s">
-        <v>19</v>
-      </c>
-      <c r="AM17" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="18" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>23</v>
-      </c>
-      <c r="C18">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="D18">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F18">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="L18">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="U18">
-        <f t="shared" si="3"/>
-        <v>12</v>
-      </c>
-      <c r="W18">
-        <v>1</v>
-      </c>
-      <c r="X18">
-        <v>1</v>
-      </c>
-      <c r="Y18">
-        <v>1</v>
-      </c>
-      <c r="Z18">
-        <v>1</v>
-      </c>
-      <c r="AB18">
-        <v>1</v>
-      </c>
-      <c r="AC18">
-        <v>1</v>
-      </c>
-      <c r="AK18" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="19" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>2</v>
       </c>
       <c r="C19">
-        <f t="shared" si="0"/>
-        <v>40</v>
+        <f>D19+X19+W19</f>
+        <v>58</v>
       </c>
       <c r="D19">
-        <f t="shared" si="1"/>
-        <v>23</v>
+        <f>SUM(E19,F19,L19,Q19,U19,V19)</f>
+        <v>37</v>
       </c>
       <c r="E19">
         <v>2</v>
       </c>
       <c r="F19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="G19">
@@ -2824,7 +3009,7 @@
         <v>0</v>
       </c>
       <c r="L19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="M19">
@@ -2839,18 +3024,25 @@
       <c r="P19">
         <v>2</v>
       </c>
+      <c r="Q19">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="R19">
+        <v>4</v>
+      </c>
+      <c r="S19">
+        <v>5</v>
+      </c>
       <c r="T19">
-        <v>1</v>
-      </c>
-      <c r="U19">
-        <f t="shared" si="3"/>
-        <v>16</v>
-      </c>
-      <c r="V19">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="W19">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="X19">
+        <f t="shared" si="2"/>
+        <v>18</v>
       </c>
       <c r="Y19">
         <v>1</v>
@@ -2858,9 +3050,6 @@
       <c r="Z19">
         <v>1</v>
       </c>
-      <c r="AA19">
-        <v>1</v>
-      </c>
       <c r="AB19">
         <v>1</v>
       </c>
@@ -2870,23 +3059,27 @@
       <c r="AD19">
         <v>1</v>
       </c>
-      <c r="AK19" t="s">
+      <c r="AE19">
+        <v>1</v>
+      </c>
+      <c r="AF19">
+        <v>1</v>
+      </c>
+      <c r="AG19">
+        <v>1</v>
+      </c>
+      <c r="AH19">
+        <v>1</v>
+      </c>
+      <c r="AN19" t="s">
         <v>10</v>
       </c>
-      <c r="AM19" t="s">
+      <c r="AP19" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="W21" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="22" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="W22" t="s">
-        <v>70</v>
-      </c>
-      <c r="X22" s="1"/>
+    <row r="22" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AA22" s="1"/>
     </row>
   </sheetData>
   <sortState ref="A6:M19">

</xml_diff>